<commit_message>
update embassy backend process
</commit_message>
<xml_diff>
--- a/public/s3/embassies-sheet.xlsx
+++ b/public/s3/embassies-sheet.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>Embassy of</t>
-  </si>
-  <si>
     <t>Embassy In</t>
   </si>
   <si>
@@ -40,6 +37,9 @@
   </si>
   <si>
     <t xml:space="preserve">contact us </t>
+  </si>
+  <si>
+    <t>Embassy City</t>
   </si>
 </sst>
 </file>
@@ -381,9 +381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:J10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -399,25 +397,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>